<commit_message>
fix (TM for Lena): Now the n_top_words param is passed to the lda_topic_modeling funciton call
</commit_message>
<xml_diff>
--- a/topic_top_words.xlsx
+++ b/topic_top_words.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -582,410 +582,410 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>sowi</t>
+          <t>entwicklung</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.009650099091231823</v>
+        <v>0.003417749656364322</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>entwickelt</t>
+          <t>bereich</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.006488995626568794</v>
+        <v>0.003339486662298441</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>projekt</t>
+          <t>bereit</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.005740313325077295</v>
+        <v>0.003339486662298441</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>sollen</t>
+          <t>foku</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.005740313325077295</v>
+        <v>0.003235135925933719</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>einsatz</t>
+          <t>ermöglicht</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.004617290105670691</v>
+        <v>0.003182960441336036</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ammoniak</t>
+          <t>informationen</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.004450916312634945</v>
+        <v>0.002974258968606591</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>rahmen</t>
+          <t>digitalen</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.004367729648947716</v>
+        <v>0.002922083484008908</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>entwicklung</t>
+          <t>sowohl</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.00420135585591197</v>
+        <v>0.002895995741710067</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>wasserstoff</t>
+          <t>system</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.004159762058407068</v>
+        <v>0.002869908232241869</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ziel</t>
+          <t>einsatz</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.003785421140491962</v>
+        <v>0.002661206526681781</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>entwicklung</t>
+          <t>sowi</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.009786198846995831</v>
+        <v>0.009650099091231823</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ziel</t>
+          <t>entwickelt</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.008428337052464485</v>
+        <v>0.006488995626568794</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>teilvorhaben</t>
+          <t>projekt</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.008241046220064163</v>
+        <v>0.005740313325077295</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>sowi</t>
+          <t>sollen</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.00746846990659833</v>
+        <v>0.005740313325077295</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>sollen</t>
+          <t>einsatz</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.006391545757651329</v>
+        <v>0.004617290105670691</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>vorhaben</t>
+          <t>ammoniak</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.005665792152285576</v>
+        <v>0.004450916312634945</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>dabei</t>
+          <t>rahmen</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.004729336127638817</v>
+        <v>0.004367729648947716</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>entwickelt</t>
+          <t>entwicklung</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.004565456416457891</v>
+        <v>0.00420135585591197</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>anforderungen</t>
+          <t>wasserstoff</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.004518633708357811</v>
+        <v>0.004159762058407068</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>eigenschaften</t>
+          <t>ziel</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.003605589270591736</v>
+        <v>0.003785421140491962</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ziel</t>
+          <t>dabei</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.00852749589830637</v>
+        <v>0.003743827575817704</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>sowi</t>
+          <t>teilvorhaben</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.008337398059666157</v>
+        <v>0.003743827575817704</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>projekt</t>
+          <t>cf</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.006273483857512474</v>
+        <v>0.003619047114625573</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>entwicklung</t>
+          <t>konzept</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.005947602912783623</v>
+        <v>0.003161519067361951</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>sollen</t>
+          <t>ua</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.005567408166825771</v>
+        <v>0.002953551709651947</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>produkt</t>
+          <t>mittel</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.00518721342086792</v>
+        <v>0.002953551709651947</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>verfahren</t>
+          <t>betrieb</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.004997116047888994</v>
+        <v>0.002911958377808332</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>herstellung</t>
+          <t>•</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.004372510593384504</v>
+        <v>0.002911958377808332</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>teilvorhaben</t>
+          <t>energi</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.004345353692770004</v>
+        <v>0.002870364813134074</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>dabei</t>
+          <t>nutzung</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.003965158946812153</v>
+        <v>0.002662397688254714</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>region</t>
+          <t>entwicklung</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.01281567104160786</v>
+        <v>0.009786198846995831</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -993,111 +993,761 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.01006728317588568</v>
+        <v>0.008428337052464485</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>sowi</t>
+          <t>teilvorhaben</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.009357025846838951</v>
+        <v>0.008241046220064163</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>entwicklung</t>
+          <t>sowi</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.008816612884402275</v>
+        <v>0.00746846990659833</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>vorhaben</t>
+          <t>sollen</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.006253509316593409</v>
+        <v>0.006391545757651329</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>projekt</t>
+          <t>vorhaben</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.005960141774266958</v>
+        <v>0.005665792152285576</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>regional</t>
+          <t>dabei</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.005620453506708145</v>
+        <v>0.004729336127638817</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>unternehmen</t>
+          <t>entwickelt</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.005249884445220232</v>
+        <v>0.004565456416457891</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>innov</t>
+          <t>anforderungen</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.005126361269503832</v>
+        <v>0.004518633708357811</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>eigenschaften</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>0.003605589270591736</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>2</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>einsatz</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>0.003605589270591736</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>2</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>gmbh</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>0.003511943621560931</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>2</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>mittel</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>0.003488532267510891</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>2</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>system</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>0.003371475264430046</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>2</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>verfahren</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>0.003254418261349201</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>2</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>fertigung</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>0.003254418261349201</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>2</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>projekt</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>0.003160772612318397</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>2</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>rahmen</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>0.003043715609237552</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>2</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>teilprojekt</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>0.003043715609237552</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>2</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>basi</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>0.003043715609237552</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>3</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ziel</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>0.00852749589830637</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>3</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>sowi</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0.008337398059666157</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>projekt</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>0.006273483857512474</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>3</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>entwicklung</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>0.005947602912783623</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>sollen</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>0.005567408166825771</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>3</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>produkt</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0.00518721342086792</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>3</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>verfahren</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0.004997116047888994</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>3</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>herstellung</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0.004372510593384504</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>3</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>teilvorhaben</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0.004345353692770004</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>3</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>dabei</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>0.003965158946812153</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>3</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>nutzung</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>0.003775061573833227</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>3</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>untersucht</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>0.003775061573833227</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>3</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>region</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0.003530650865286589</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>3</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>rohstoff</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0.003422023961320519</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>3</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>entwickelt</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>0.003367710392922163</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>3</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>einsatz</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>0.003204769920557737</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>3</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>zb</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>0.003068985883146524</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>3</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>aufbereitung</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>0.003041829215362668</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>3</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>rahmen</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>0.003014672547578812</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>3</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>reststoff</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>0.003014672547578812</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>4</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>region</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>0.01281567104160786</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>4</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>ziel</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>0.01006728317588568</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>4</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>sowi</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>0.009357025846838951</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>4</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>entwicklung</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>0.008816612884402275</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>4</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>vorhaben</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>0.006253509316593409</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>4</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>projekt</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>0.005960141774266958</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>4</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>regional</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>0.005620453506708145</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>4</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>unternehmen</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>0.005249884445220232</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>4</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>innov</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>0.005126361269503832</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>4</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
           <t>neue</t>
         </is>
       </c>
-      <c r="C51" t="n">
+      <c r="C91" t="n">
         <v>0.004647709429264069</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>4</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>bündniss</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>0.004416103940457106</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>4</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>sollen</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>0.004369782749563456</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>4</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>regionalen</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>0.004369782749563456</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>4</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>bündni</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>0.004292580764740705</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>4</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>nachhaltig</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>0.004107296001166105</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>4</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>dabei</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>0.003505120985209942</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>4</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>konzept</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>0.003505120985209942</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>4</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>umsetzung</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>0.003273515263572335</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>4</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>rahmen</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>0.003242634469643235</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>4</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>entwickeln</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>0.003196313278749585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>